<commit_message>
Removed old code and added extractions folder for excel list exports
</commit_message>
<xml_diff>
--- a/TP.xlsx
+++ b/TP.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/2021-June_Mote/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_EE62FDCE8F79A8D366075C52F3E662B6561AA196" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1DB1853-5E00-4C98-B34A-8DBAFCF42178}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1464" yWindow="1248" windowWidth="11196" windowHeight="11808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,14 +63,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -123,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -155,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,16 +350,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>T0</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>T4</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>T5</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TF</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>